<commit_message>
arreglo script de validacion SISE en PREPROD
</commit_message>
<xml_diff>
--- a/SuraClaims/AprobacionesPreviasAPago.xlsx
+++ b/SuraClaims/AprobacionesPreviasAPago.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Irina Storozuk\Documents\Ranorex\RanorexStudio Projects\SuraClaims\SuraClaims\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43D47640-01CD-4047-9853-73E39591B0FF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79C3EFD3-8303-4B58-84EA-EE1662210EDD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D25DB973-7044-4683-AF33-2EEB0F8C9B88}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>Ambiente</t>
   </si>
@@ -54,14 +54,23 @@
     <t>https://ssurgwsoadev4-oci.opc.oracleoutsourcing.com/cc/ClaimCenter.do</t>
   </si>
   <si>
-    <t>1220194200610</t>
+    <t>1120170200906</t>
+  </si>
+  <si>
+    <t>i-preproducciongestion.segurossura.com.ar</t>
+  </si>
+  <si>
+    <t>https://i-preproducciongestion.segurossura.com.ar/cc/ClaimCenter.do</t>
+  </si>
+  <si>
+    <t>1120170200907</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -74,6 +83,14 @@
       <color theme="1"/>
       <name val="Segoe UI"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -93,16 +110,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -415,10 +436,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C9B9E65-C06E-45A4-A7F6-A46B8429DFA4}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -457,7 +478,27 @@
         <v>9</v>
       </c>
     </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{9F85603E-8947-41C3-AEF4-568B0E25B994}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
agrego preguntas de siniestro motor para aprobaciones previas a pago
</commit_message>
<xml_diff>
--- a/SuraClaims/AprobacionesPreviasAPago.xlsx
+++ b/SuraClaims/AprobacionesPreviasAPago.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Irina Storozuk\Documents\Ranorex\RanorexStudio Projects\SuraClaims\SuraClaims\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B4E132C-F10B-4A22-9EE1-3DFC432C8697}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90317DCA-1B9C-4E9D-8396-8E4CCE821145}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D25DB973-7044-4683-AF33-2EEB0F8C9B88}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="18">
   <si>
     <t>Ambiente</t>
   </si>
@@ -73,6 +73,12 @@
   </si>
   <si>
     <t xml:space="preserve">1220170301429   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">0420194406715 </t>
+  </si>
+  <si>
+    <t>mgentilini</t>
   </si>
 </sst>
 </file>
@@ -445,10 +451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C9B9E65-C06E-45A4-A7F6-A46B8429DFA4}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -470,7 +476,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="28.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -478,13 +484,13 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="D2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>13</v>
+      <c r="E2" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="28.5" x14ac:dyDescent="0.25">
@@ -501,15 +507,15 @@
         <v>4</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
@@ -517,8 +523,8 @@
       <c r="D4" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>15</v>
+      <c r="E4" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -529,19 +535,36 @@
         <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D5" t="s">
         <v>4</v>
       </c>
       <c r="E5" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>14</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B5" r:id="rId1" xr:uid="{9F85603E-8947-41C3-AEF4-568B0E25B994}"/>
-    <hyperlink ref="B4" r:id="rId2" xr:uid="{45A517EF-F937-4CF3-9BC2-F4E43A955B11}"/>
+    <hyperlink ref="B6" r:id="rId1" xr:uid="{9F85603E-8947-41C3-AEF4-568B0E25B994}"/>
+    <hyperlink ref="B5" r:id="rId2" xr:uid="{45A517EF-F937-4CF3-9BC2-F4E43A955B11}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>